<commit_message>
update responsabilidades e planeamento
</commit_message>
<xml_diff>
--- a/Documentacao/matriz de responsabilidades V2.xlsx
+++ b/Documentacao/matriz de responsabilidades V2.xlsx
@@ -610,7 +610,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
@@ -702,6 +702,19 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1010,8 +1023,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="B36" sqref="B36"/>
+    <sheetView tabSelected="1" topLeftCell="A42" workbookViewId="0">
+      <selection activeCell="F54" sqref="F54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1472,7 +1485,9 @@
       <c r="D26" s="5">
         <v>1</v>
       </c>
-      <c r="E26" s="5"/>
+      <c r="E26" s="5">
+        <v>1</v>
+      </c>
       <c r="F26" s="10"/>
     </row>
     <row r="27" spans="1:6" s="24" customFormat="1" x14ac:dyDescent="0.25">
@@ -1578,16 +1593,14 @@
       <c r="B33" s="13" t="s">
         <v>77</v>
       </c>
-      <c r="C33" s="7">
-        <v>1</v>
-      </c>
+      <c r="C33" s="7"/>
       <c r="D33" s="7">
         <v>1</v>
       </c>
-      <c r="E33" s="7">
-        <v>1</v>
-      </c>
-      <c r="F33" s="8"/>
+      <c r="E33" s="7"/>
+      <c r="F33" s="8">
+        <v>1</v>
+      </c>
     </row>
     <row r="34" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34" s="20" t="s">
@@ -1599,7 +1612,9 @@
       <c r="C34" s="9">
         <v>1</v>
       </c>
-      <c r="D34" s="9"/>
+      <c r="D34" s="9">
+        <v>1</v>
+      </c>
       <c r="E34" s="9">
         <v>1</v>
       </c>
@@ -1635,7 +1650,9 @@
       <c r="E36" s="5">
         <v>2</v>
       </c>
-      <c r="F36" s="10"/>
+      <c r="F36" s="10">
+        <v>3</v>
+      </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" s="19" t="s">
@@ -1660,14 +1677,14 @@
       <c r="B38" s="14" t="s">
         <v>84</v>
       </c>
-      <c r="C38" s="5">
-        <v>1</v>
-      </c>
+      <c r="C38" s="5"/>
       <c r="D38" s="5"/>
       <c r="E38" s="5">
         <v>1</v>
       </c>
-      <c r="F38" s="10"/>
+      <c r="F38" s="10">
+        <v>1</v>
+      </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" s="19" t="s">
@@ -1685,7 +1702,9 @@
       <c r="E39" s="7">
         <v>1</v>
       </c>
-      <c r="F39" s="8"/>
+      <c r="F39" s="8">
+        <v>3</v>
+      </c>
     </row>
     <row r="40" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A40" s="20" t="s">
@@ -1703,7 +1722,9 @@
       <c r="E40" s="9">
         <v>1</v>
       </c>
-      <c r="F40" s="10"/>
+      <c r="F40" s="10">
+        <v>3</v>
+      </c>
     </row>
     <row r="41" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A41" s="19" t="s">
@@ -1785,19 +1806,19 @@
         <v>30</v>
       </c>
     </row>
-    <row r="46" spans="1:6" s="29" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="18" t="s">
+    <row r="46" spans="1:6" s="39" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="20" t="s">
         <v>95</v>
       </c>
-      <c r="B46" s="12" t="s">
+      <c r="B46" s="14" t="s">
         <v>96</v>
       </c>
-      <c r="C46" s="31">
-        <v>1</v>
-      </c>
-      <c r="D46" s="31"/>
-      <c r="E46" s="31"/>
-      <c r="F46" s="32"/>
+      <c r="C46" s="37">
+        <v>1</v>
+      </c>
+      <c r="D46" s="37"/>
+      <c r="E46" s="37"/>
+      <c r="F46" s="38"/>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" s="19" t="s">
@@ -1825,7 +1846,9 @@
       <c r="E48" s="5">
         <v>1</v>
       </c>
-      <c r="F48" s="6"/>
+      <c r="F48" s="6">
+        <v>1</v>
+      </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" s="19" t="s">
@@ -1839,7 +1862,9 @@
       <c r="E49" s="7">
         <v>1</v>
       </c>
-      <c r="F49" s="8"/>
+      <c r="F49" s="8">
+        <v>1</v>
+      </c>
     </row>
     <row r="50" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A50" s="20" t="s">
@@ -1871,7 +1896,9 @@
         <v>1</v>
       </c>
       <c r="E51" s="7"/>
-      <c r="F51" s="8"/>
+      <c r="F51" s="8">
+        <v>1</v>
+      </c>
     </row>
     <row r="52" spans="1:6" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A52" s="20" t="s">
@@ -1887,39 +1914,41 @@
       <c r="E52" s="9"/>
       <c r="F52" s="10"/>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A53" s="19" t="s">
+    <row r="53" spans="1:6" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A53" s="21" t="s">
         <v>109</v>
       </c>
-      <c r="B53" s="13" t="s">
+      <c r="B53" s="15" t="s">
         <v>110</v>
       </c>
-      <c r="C53" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="D53" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="E53" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="F53" s="8" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="54" spans="1:6" s="29" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="18" t="s">
+      <c r="C53" s="40" t="s">
+        <v>30</v>
+      </c>
+      <c r="D53" s="40" t="s">
+        <v>30</v>
+      </c>
+      <c r="E53" s="40" t="s">
+        <v>30</v>
+      </c>
+      <c r="F53" s="41" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" s="39" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A54" s="20" t="s">
         <v>111</v>
       </c>
-      <c r="B54" s="12" t="s">
+      <c r="B54" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="C54" s="31"/>
-      <c r="D54" s="31">
-        <v>1</v>
-      </c>
-      <c r="E54" s="31"/>
-      <c r="F54" s="32"/>
+      <c r="C54" s="37"/>
+      <c r="D54" s="37">
+        <v>1</v>
+      </c>
+      <c r="E54" s="37"/>
+      <c r="F54" s="38">
+        <v>1</v>
+      </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55" s="19" t="s">

</xml_diff>